<commit_message>
CPUTester: Still not working
</commit_message>
<xml_diff>
--- a/Related/assembler_table.xlsx
+++ b/Related/assembler_table.xlsx
@@ -190,7 +190,7 @@
     <t xml:space="preserve">No Operation</t>
   </si>
   <si>
-    <t xml:space="preserve">COMP Rx, Ry</t>
+    <t xml:space="preserve">CMP Rx, Ry</t>
   </si>
   <si>
     <t xml:space="preserve">Compare / Test</t>
@@ -572,8 +572,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C75" activeCellId="0" sqref="C75"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F32" activeCellId="0" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.9296875" defaultRowHeight="41.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1849,7 +1849,7 @@
         <v>44</v>
       </c>
       <c r="F37" s="10" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="G37" s="10" t="s">
         <v>18</v>
@@ -1946,19 +1946,19 @@
         <v>44</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="H40" s="6" t="s">
         <v>17</v>
       </c>
       <c r="I40" s="6" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="J40" s="6" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="K40" s="6" t="s">
         <v>62</v>
@@ -1986,19 +1986,19 @@
         <v>44</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="G41" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="H41" s="8" t="s">
         <v>17</v>
       </c>
       <c r="I41" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="J41" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="K41" s="8" t="s">
         <v>64</v>
@@ -2026,19 +2026,19 @@
         <v>44</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="H42" s="8" t="s">
         <v>17</v>
       </c>
       <c r="I42" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="J42" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="K42" s="8" t="s">
         <v>66</v>
@@ -2066,19 +2066,19 @@
         <v>44</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="H43" s="8" t="s">
         <v>17</v>
       </c>
       <c r="I43" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="J43" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="K43" s="8" t="s">
         <v>68</v>
@@ -2106,19 +2106,19 @@
         <v>44</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="G44" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="H44" s="8" t="s">
         <v>17</v>
       </c>
       <c r="I44" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="J44" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="K44" s="8" t="s">
         <v>70</v>
@@ -2146,19 +2146,19 @@
         <v>44</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="G45" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="H45" s="8" t="s">
         <v>17</v>
       </c>
       <c r="I45" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="J45" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="K45" s="8" t="s">
         <v>72</v>
@@ -2186,19 +2186,19 @@
         <v>44</v>
       </c>
       <c r="F46" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="G46" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="H46" s="8" t="s">
         <v>17</v>
       </c>
       <c r="I46" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="J46" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="K46" s="8" t="s">
         <v>74</v>
@@ -2226,19 +2226,19 @@
         <v>44</v>
       </c>
       <c r="F47" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="G47" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="H47" s="8" t="s">
         <v>17</v>
       </c>
       <c r="I47" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="J47" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="K47" s="8" t="s">
         <v>76</v>
@@ -2266,19 +2266,19 @@
         <v>44</v>
       </c>
       <c r="F48" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="G48" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="H48" s="8" t="s">
         <v>17</v>
       </c>
       <c r="I48" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="J48" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="K48" s="8" t="s">
         <v>78</v>
@@ -2306,19 +2306,19 @@
         <v>44</v>
       </c>
       <c r="F49" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="G49" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="H49" s="8" t="s">
         <v>17</v>
       </c>
       <c r="I49" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="J49" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="K49" s="8" t="s">
         <v>80</v>
@@ -2346,19 +2346,19 @@
         <v>44</v>
       </c>
       <c r="F50" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="G50" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="H50" s="8" t="s">
         <v>17</v>
       </c>
       <c r="I50" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="J50" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="K50" s="8" t="s">
         <v>82</v>
@@ -2386,19 +2386,19 @@
         <v>44</v>
       </c>
       <c r="F51" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="G51" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="H51" s="8" t="s">
         <v>17</v>
       </c>
       <c r="I51" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="J51" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="K51" s="8" t="s">
         <v>84</v>
@@ -2426,19 +2426,19 @@
         <v>44</v>
       </c>
       <c r="F52" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="G52" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="H52" s="8" t="s">
         <v>17</v>
       </c>
       <c r="I52" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="J52" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="K52" s="8" t="s">
         <v>86</v>
@@ -2466,19 +2466,19 @@
         <v>44</v>
       </c>
       <c r="F53" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="G53" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="H53" s="8" t="s">
         <v>17</v>
       </c>
       <c r="I53" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="J53" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="K53" s="8" t="s">
         <v>88</v>
@@ -2506,19 +2506,19 @@
         <v>44</v>
       </c>
       <c r="F54" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="G54" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="H54" s="8" t="s">
         <v>17</v>
       </c>
       <c r="I54" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="J54" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="K54" s="8" t="s">
         <v>90</v>
@@ -2546,19 +2546,19 @@
         <v>44</v>
       </c>
       <c r="F55" s="10" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="G55" s="10" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="H55" s="10" t="s">
         <v>17</v>
       </c>
       <c r="I55" s="10" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="J55" s="10" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="K55" s="10" t="s">
         <v>92</v>
@@ -2658,7 +2658,7 @@
         <v>44</v>
       </c>
       <c r="F59" s="6" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="G59" s="5" t="s">
         <v>41</v>
@@ -2692,7 +2692,7 @@
         <v>44</v>
       </c>
       <c r="F60" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="G60" s="7" t="s">
         <v>41</v>
@@ -2726,7 +2726,7 @@
         <v>44</v>
       </c>
       <c r="F61" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="G61" s="7" t="s">
         <v>41</v>
@@ -2760,7 +2760,7 @@
         <v>44</v>
       </c>
       <c r="F62" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="G62" s="7" t="s">
         <v>41</v>
@@ -2794,7 +2794,7 @@
         <v>44</v>
       </c>
       <c r="F63" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="G63" s="7" t="s">
         <v>41</v>
@@ -2828,7 +2828,7 @@
         <v>44</v>
       </c>
       <c r="F64" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="G64" s="7" t="s">
         <v>41</v>
@@ -2862,7 +2862,7 @@
         <v>44</v>
       </c>
       <c r="F65" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="G65" s="7" t="s">
         <v>41</v>
@@ -2896,7 +2896,7 @@
         <v>44</v>
       </c>
       <c r="F66" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="G66" s="7" t="s">
         <v>41</v>
@@ -2930,7 +2930,7 @@
         <v>44</v>
       </c>
       <c r="F67" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="G67" s="7" t="s">
         <v>41</v>
@@ -2964,7 +2964,7 @@
         <v>44</v>
       </c>
       <c r="F68" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="G68" s="7" t="s">
         <v>41</v>
@@ -2998,7 +2998,7 @@
         <v>44</v>
       </c>
       <c r="F69" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="G69" s="7" t="s">
         <v>41</v>
@@ -3032,7 +3032,7 @@
         <v>44</v>
       </c>
       <c r="F70" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="G70" s="7" t="s">
         <v>41</v>
@@ -3066,7 +3066,7 @@
         <v>44</v>
       </c>
       <c r="F71" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="G71" s="7" t="s">
         <v>41</v>
@@ -4110,7 +4110,7 @@
         <v>44</v>
       </c>
       <c r="F72" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="G72" s="7" t="s">
         <v>41</v>
@@ -5154,7 +5154,7 @@
         <v>44</v>
       </c>
       <c r="F73" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="G73" s="7" t="s">
         <v>41</v>
@@ -6198,7 +6198,7 @@
         <v>44</v>
       </c>
       <c r="F74" s="10" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="G74" s="9" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
Fixed a bug in assembler
</commit_message>
<xml_diff>
--- a/Related/assembler_table.xlsx
+++ b/Related/assembler_table.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="109">
   <si>
     <t xml:space="preserve">Command Table</t>
   </si>
@@ -362,6 +362,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -382,29 +383,34 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="24"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -572,11 +578,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F32" activeCellId="0" sqref="F32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I76" activeCellId="0" sqref="I76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="21.9296875" defaultRowHeight="41.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="21.921875" defaultRowHeight="41.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="1" width="21.9"/>
   </cols>
@@ -2660,12 +2666,14 @@
       <c r="F59" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G59" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="H59" s="5"/>
-      <c r="I59" s="5"/>
-      <c r="J59" s="5"/>
+      <c r="G59" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H59" s="6"/>
+      <c r="I59" s="6"/>
+      <c r="J59" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="K59" s="6" t="s">
         <v>62</v>
       </c>
@@ -2694,12 +2702,14 @@
       <c r="F60" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="G60" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="H60" s="7"/>
-      <c r="I60" s="7"/>
-      <c r="J60" s="7"/>
+      <c r="G60" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H60" s="8"/>
+      <c r="I60" s="8"/>
+      <c r="J60" s="7" t="s">
+        <v>18</v>
+      </c>
       <c r="K60" s="8" t="s">
         <v>64</v>
       </c>
@@ -2728,12 +2738,14 @@
       <c r="F61" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="G61" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="H61" s="7"/>
-      <c r="I61" s="7"/>
-      <c r="J61" s="7"/>
+      <c r="G61" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H61" s="8"/>
+      <c r="I61" s="8"/>
+      <c r="J61" s="7" t="s">
+        <v>18</v>
+      </c>
       <c r="K61" s="8" t="s">
         <v>66</v>
       </c>
@@ -2762,12 +2774,14 @@
       <c r="F62" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="G62" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="H62" s="7"/>
-      <c r="I62" s="7"/>
-      <c r="J62" s="7"/>
+      <c r="G62" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H62" s="8"/>
+      <c r="I62" s="8"/>
+      <c r="J62" s="7" t="s">
+        <v>18</v>
+      </c>
       <c r="K62" s="8" t="s">
         <v>68</v>
       </c>
@@ -2796,12 +2810,14 @@
       <c r="F63" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="G63" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="H63" s="7"/>
-      <c r="I63" s="7"/>
-      <c r="J63" s="7"/>
+      <c r="G63" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H63" s="8"/>
+      <c r="I63" s="8"/>
+      <c r="J63" s="7" t="s">
+        <v>18</v>
+      </c>
       <c r="K63" s="8" t="s">
         <v>70</v>
       </c>
@@ -2830,12 +2846,14 @@
       <c r="F64" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="G64" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="H64" s="7"/>
-      <c r="I64" s="7"/>
-      <c r="J64" s="7"/>
+      <c r="G64" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H64" s="8"/>
+      <c r="I64" s="8"/>
+      <c r="J64" s="7" t="s">
+        <v>18</v>
+      </c>
       <c r="K64" s="8" t="s">
         <v>72</v>
       </c>
@@ -2864,12 +2882,14 @@
       <c r="F65" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="G65" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="H65" s="7"/>
-      <c r="I65" s="7"/>
-      <c r="J65" s="7"/>
+      <c r="G65" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H65" s="8"/>
+      <c r="I65" s="8"/>
+      <c r="J65" s="7" t="s">
+        <v>18</v>
+      </c>
       <c r="K65" s="8" t="s">
         <v>74</v>
       </c>
@@ -2898,12 +2918,14 @@
       <c r="F66" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="G66" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="H66" s="7"/>
-      <c r="I66" s="7"/>
-      <c r="J66" s="7"/>
+      <c r="G66" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H66" s="8"/>
+      <c r="I66" s="8"/>
+      <c r="J66" s="7" t="s">
+        <v>18</v>
+      </c>
       <c r="K66" s="8" t="s">
         <v>76</v>
       </c>
@@ -2932,12 +2954,14 @@
       <c r="F67" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="G67" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="H67" s="7"/>
-      <c r="I67" s="7"/>
-      <c r="J67" s="7"/>
+      <c r="G67" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H67" s="8"/>
+      <c r="I67" s="8"/>
+      <c r="J67" s="7" t="s">
+        <v>18</v>
+      </c>
       <c r="K67" s="8" t="s">
         <v>78</v>
       </c>
@@ -2966,12 +2990,14 @@
       <c r="F68" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="G68" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="H68" s="7"/>
-      <c r="I68" s="7"/>
-      <c r="J68" s="7"/>
+      <c r="G68" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H68" s="8"/>
+      <c r="I68" s="8"/>
+      <c r="J68" s="7" t="s">
+        <v>18</v>
+      </c>
       <c r="K68" s="8" t="s">
         <v>80</v>
       </c>
@@ -3000,12 +3026,14 @@
       <c r="F69" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="G69" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="H69" s="7"/>
-      <c r="I69" s="7"/>
-      <c r="J69" s="7"/>
+      <c r="G69" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H69" s="8"/>
+      <c r="I69" s="8"/>
+      <c r="J69" s="7" t="s">
+        <v>18</v>
+      </c>
       <c r="K69" s="8" t="s">
         <v>82</v>
       </c>
@@ -3034,12 +3062,14 @@
       <c r="F70" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="G70" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="H70" s="7"/>
-      <c r="I70" s="7"/>
-      <c r="J70" s="7"/>
+      <c r="G70" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H70" s="8"/>
+      <c r="I70" s="8"/>
+      <c r="J70" s="7" t="s">
+        <v>18</v>
+      </c>
       <c r="K70" s="8" t="s">
         <v>84</v>
       </c>
@@ -3068,12 +3098,14 @@
       <c r="F71" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="G71" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="H71" s="7"/>
-      <c r="I71" s="7"/>
-      <c r="J71" s="7"/>
+      <c r="G71" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H71" s="8"/>
+      <c r="I71" s="8"/>
+      <c r="J71" s="7" t="s">
+        <v>18</v>
+      </c>
       <c r="K71" s="8" t="s">
         <v>86</v>
       </c>
@@ -4112,12 +4144,14 @@
       <c r="F72" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="G72" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="H72" s="7"/>
-      <c r="I72" s="7"/>
-      <c r="J72" s="7"/>
+      <c r="G72" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H72" s="8"/>
+      <c r="I72" s="8"/>
+      <c r="J72" s="7" t="s">
+        <v>18</v>
+      </c>
       <c r="K72" s="8" t="s">
         <v>88</v>
       </c>
@@ -5156,12 +5190,14 @@
       <c r="F73" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="G73" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="H73" s="7"/>
-      <c r="I73" s="7"/>
-      <c r="J73" s="7"/>
+      <c r="G73" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H73" s="8"/>
+      <c r="I73" s="8"/>
+      <c r="J73" s="7" t="s">
+        <v>18</v>
+      </c>
       <c r="K73" s="8" t="s">
         <v>90</v>
       </c>
@@ -6200,12 +6236,14 @@
       <c r="F74" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="G74" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="H74" s="9"/>
-      <c r="I74" s="9"/>
-      <c r="J74" s="9"/>
+      <c r="G74" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="H74" s="10"/>
+      <c r="I74" s="10"/>
+      <c r="J74" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="K74" s="10" t="s">
         <v>92</v>
       </c>
@@ -7254,22 +7292,22 @@
     <mergeCell ref="G31:I31"/>
     <mergeCell ref="G32:I32"/>
     <mergeCell ref="B57:M57"/>
-    <mergeCell ref="G59:J59"/>
-    <mergeCell ref="G60:J60"/>
-    <mergeCell ref="G61:J61"/>
-    <mergeCell ref="G62:J62"/>
-    <mergeCell ref="G63:J63"/>
-    <mergeCell ref="G64:J64"/>
-    <mergeCell ref="G65:J65"/>
-    <mergeCell ref="G66:J66"/>
-    <mergeCell ref="G67:J67"/>
-    <mergeCell ref="G68:J68"/>
-    <mergeCell ref="G69:J69"/>
-    <mergeCell ref="G70:J70"/>
-    <mergeCell ref="G71:J71"/>
-    <mergeCell ref="G72:J72"/>
-    <mergeCell ref="G73:J73"/>
-    <mergeCell ref="G74:J74"/>
+    <mergeCell ref="G59:I59"/>
+    <mergeCell ref="G60:I60"/>
+    <mergeCell ref="G61:I61"/>
+    <mergeCell ref="G62:I62"/>
+    <mergeCell ref="G63:I63"/>
+    <mergeCell ref="G64:I64"/>
+    <mergeCell ref="G65:I65"/>
+    <mergeCell ref="G66:I66"/>
+    <mergeCell ref="G67:I67"/>
+    <mergeCell ref="G68:I68"/>
+    <mergeCell ref="G69:I69"/>
+    <mergeCell ref="G70:I70"/>
+    <mergeCell ref="G71:I71"/>
+    <mergeCell ref="G72:I72"/>
+    <mergeCell ref="G73:I73"/>
+    <mergeCell ref="G74:I74"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>